<commit_message>
nieuwe map en md gemaakt, moet nog retrofitten in md-comments
</commit_message>
<xml_diff>
--- a/maps/Admission-Encounter.xlsx
+++ b/maps/Admission-Encounter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/jacob_engel_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{C7E22464-8063-5A48-8AF8-B8CBF9685F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDA904EF-321F-614F-BB1E-2CA2B2C1164D}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{C7E22464-8063-5A48-8AF8-B8CBF9685F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4358876-6819-6A41-AE71-617FC158CF6C}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="780" windowWidth="16560" windowHeight="22660" xr2:uid="{4D4295CA-5E27-D54A-800A-CCB7595BF199}"/>
+    <workbookView xWindow="720" yWindow="780" windowWidth="20400" windowHeight="22660" xr2:uid="{4D4295CA-5E27-D54A-800A-CCB7595BF199}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81200B0-CEC8-5048-84D0-94AD3B33B9B6}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,9 +842,6 @@
       <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B39" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
@@ -854,6 +851,9 @@
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>